<commit_message>
fixing a manual audit flag
</commit_message>
<xml_diff>
--- a/fastqFiles/fastq_3016.xlsx
+++ b/fastqFiles/fastq_3016.xlsx
@@ -183,7 +183,7 @@
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F7" activeCellId="0" sqref="F7"/>
+      <selection pane="topLeft" activeCell="H7" activeCellId="0" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -354,7 +354,7 @@
         <v>18</v>
       </c>
       <c r="H7" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I7" s="0" t="s">
         <v>19</v>

</xml_diff>